<commit_message>
starting graphs for varying temps
also minor adjustments
</commit_message>
<xml_diff>
--- a/polynomial calcs.xlsx
+++ b/polynomial calcs.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\embas\Documents\GitHub\Thermal-Fluids-Gas-Turbine-Simulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50B2E216-88C3-459B-954A-4BCC66AC3E24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{486E814F-4F20-424F-8D6A-B748ED6D57E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-83" yWindow="0" windowWidth="10965" windowHeight="12863" xr2:uid="{7ECF82CD-4B31-4C5B-B4C1-F49AFA1B0555}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{7ECF82CD-4B31-4C5B-B4C1-F49AFA1B0555}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -222,7 +222,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$B$40</c:f>
+              <c:f>Sheet1!$B$4:$B$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="36"/>
@@ -298,12 +298,48 @@
                 <c:pt idx="23">
                   <c:v>1800</c:v>
                 </c:pt>
+                <c:pt idx="24">
+                  <c:v>1900</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2200</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2400</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2600</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2700</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2800</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2900</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3000</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$5:$C$40</c:f>
+              <c:f>Sheet1!$C$4:$C$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="36"/>
@@ -378,6 +414,42 @@
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>57651</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>61220</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>64810</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>68417</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>72040</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>75676</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>79320</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>82981</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>86650</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>90328</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>94014</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>97705</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>101407</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -482,7 +554,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$B$40</c:f>
+              <c:f>Sheet1!$B$4:$B$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="36"/>
@@ -558,12 +630,48 @@
                 <c:pt idx="23">
                   <c:v>1800</c:v>
                 </c:pt>
+                <c:pt idx="24">
+                  <c:v>1900</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2200</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2400</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2600</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2700</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2800</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2900</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3000</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$5:$E$40</c:f>
+              <c:f>Sheet1!$E$4:$E$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="36"/>
@@ -638,6 +746,42 @@
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>60371</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>64116</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>67881</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>71668</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>75484</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>79316</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>83174</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>87057</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>90956</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>94881</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>98826</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>102793</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>106780</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -980,162 +1124,234 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$B$40</c:f>
+              <c:f>Sheet1!$B$4:$B$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>250</c:v>
+                </c:pt>
                 <c:pt idx="1">
-                  <c:v>250</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>300</c:v>
+                  <c:v>350</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>350</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>400</c:v>
+                  <c:v>450</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>450</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>500</c:v>
+                  <c:v>550</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>550</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>600</c:v>
+                  <c:v>650</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>650</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>700</c:v>
+                  <c:v>750</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>750</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>800</c:v>
+                  <c:v>850</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>850</c:v>
+                  <c:v>900</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>900</c:v>
+                  <c:v>950</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>950</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1000</c:v>
+                  <c:v>1100</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1100</c:v>
+                  <c:v>1200</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1200</c:v>
+                  <c:v>1300</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1300</c:v>
+                  <c:v>1400</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1400</c:v>
+                  <c:v>1500</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1500</c:v>
+                  <c:v>1600</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1600</c:v>
+                  <c:v>1700</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1700</c:v>
+                  <c:v>1800</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1800</c:v>
+                  <c:v>1900</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2200</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2400</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2600</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2700</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2800</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2900</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$4:$D$40</c:f>
+              <c:f>Sheet1!$D$4:$D$39</c:f>
               <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0" formatCode="0.000">
+                  <c:v>186.37</c:v>
+                </c:pt>
                 <c:pt idx="1">
-                  <c:v>186.37</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="General">
                   <c:v>191.68199999999999</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="General">
+                <c:pt idx="2">
                   <c:v>196.173</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="General">
+                <c:pt idx="3">
                   <c:v>200.071</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="General">
+                <c:pt idx="4">
                   <c:v>203.523</c:v>
                 </c:pt>
+                <c:pt idx="5" formatCode="0.000">
+                  <c:v>206.63</c:v>
+                </c:pt>
                 <c:pt idx="6">
-                  <c:v>206.63</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="General">
                   <c:v>209.46100000000001</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="General">
+                <c:pt idx="7">
                   <c:v>212.066</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="General">
+                <c:pt idx="8">
                   <c:v>214.489</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="General">
+                <c:pt idx="9">
                   <c:v>216.756</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="General">
+                <c:pt idx="10">
                   <c:v>218.88900000000001</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="General">
+                <c:pt idx="11">
                   <c:v>220.90700000000001</c:v>
                 </c:pt>
-                <c:pt idx="13" formatCode="General">
+                <c:pt idx="12">
                   <c:v>222.822</c:v>
                 </c:pt>
-                <c:pt idx="14" formatCode="General">
+                <c:pt idx="13">
                   <c:v>224.64699999999999</c:v>
                 </c:pt>
-                <c:pt idx="15" formatCode="General">
+                <c:pt idx="14">
                   <c:v>226.38900000000001</c:v>
                 </c:pt>
-                <c:pt idx="16" formatCode="General">
+                <c:pt idx="15">
                   <c:v>228.05699999999999</c:v>
                 </c:pt>
-                <c:pt idx="17" formatCode="General">
+                <c:pt idx="16">
                   <c:v>231.19900000000001</c:v>
                 </c:pt>
-                <c:pt idx="18" formatCode="General">
+                <c:pt idx="17">
                   <c:v>234.11500000000001</c:v>
                 </c:pt>
-                <c:pt idx="19" formatCode="General">
+                <c:pt idx="18">
                   <c:v>236.83099999999999</c:v>
                 </c:pt>
-                <c:pt idx="20" formatCode="General">
+                <c:pt idx="19">
                   <c:v>239.375</c:v>
                 </c:pt>
-                <c:pt idx="21" formatCode="General">
+                <c:pt idx="20">
                   <c:v>241.768</c:v>
                 </c:pt>
-                <c:pt idx="22" formatCode="General">
+                <c:pt idx="21">
                   <c:v>244.02799999999999</c:v>
                 </c:pt>
-                <c:pt idx="23" formatCode="General">
+                <c:pt idx="22">
                   <c:v>246.166</c:v>
                 </c:pt>
-                <c:pt idx="24" formatCode="General">
+                <c:pt idx="23">
                   <c:v>248.19499999999999</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>250.12799999999999</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>251.96899999999999</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>253.726</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>255.41200000000001</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>257.02699999999999</c:v>
+                </c:pt>
+                <c:pt idx="29" formatCode="0.000">
+                  <c:v>258.58</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>260.07299999999998</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>261.512</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>262.90199999999999</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>264.24099999999999</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>265.53800000000001</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>266.79300000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1240,162 +1456,234 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$B$40</c:f>
+              <c:f>Sheet1!$B$4:$B$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>250</c:v>
+                </c:pt>
                 <c:pt idx="1">
-                  <c:v>250</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>300</c:v>
+                  <c:v>350</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>350</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>400</c:v>
+                  <c:v>450</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>450</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>500</c:v>
+                  <c:v>550</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>550</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>600</c:v>
+                  <c:v>650</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>650</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>700</c:v>
+                  <c:v>750</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>750</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>800</c:v>
+                  <c:v>850</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>850</c:v>
+                  <c:v>900</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>900</c:v>
+                  <c:v>950</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>950</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1000</c:v>
+                  <c:v>1100</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1100</c:v>
+                  <c:v>1200</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1200</c:v>
+                  <c:v>1300</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1300</c:v>
+                  <c:v>1400</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1400</c:v>
+                  <c:v>1500</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1500</c:v>
+                  <c:v>1600</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1600</c:v>
+                  <c:v>1700</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1700</c:v>
+                  <c:v>1800</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1800</c:v>
+                  <c:v>1900</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2200</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2400</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2600</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2700</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2800</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2900</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$4:$F$40</c:f>
+              <c:f>Sheet1!$F$4:$F$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="37"/>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>199.88499999999999</c:v>
+                </c:pt>
                 <c:pt idx="1">
-                  <c:v>199.88499999999999</c:v>
+                  <c:v>205.21299999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>205.21299999999999</c:v>
+                  <c:v>209.76499999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>209.76499999999999</c:v>
+                  <c:v>213.76499999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>213.76499999999999</c:v>
+                  <c:v>217.34200000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>217.34200000000001</c:v>
+                  <c:v>220.589</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>220.589</c:v>
+                  <c:v>223.57599999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>223.57599999999999</c:v>
+                  <c:v>226.346</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>226.346</c:v>
+                  <c:v>228.93199999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>228.93199999999999</c:v>
+                  <c:v>231.358</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>231.358</c:v>
-                </c:pt>
-                <c:pt idx="11">
                   <c:v>233.649</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="0.000">
+                <c:pt idx="11" formatCode="0.000">
                   <c:v>235.81</c:v>
                 </c:pt>
+                <c:pt idx="12">
+                  <c:v>237.864</c:v>
+                </c:pt>
                 <c:pt idx="13">
-                  <c:v>237.864</c:v>
+                  <c:v>239.82300000000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>239.82300000000001</c:v>
+                  <c:v>241.68899999999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>241.68899999999999</c:v>
+                  <c:v>243.471</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>243.471</c:v>
+                  <c:v>246.81800000000001</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>246.81800000000001</c:v>
+                  <c:v>249.90600000000001</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>249.90600000000001</c:v>
+                  <c:v>252.77600000000001</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>252.77600000000001</c:v>
+                  <c:v>255.45400000000001</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>255.45400000000001</c:v>
+                  <c:v>257.96499999999997</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>257.96499999999997</c:v>
+                  <c:v>260.33300000000003</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>260.33300000000003</c:v>
+                  <c:v>262.57100000000003</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>262.57100000000003</c:v>
+                  <c:v>264.70100000000002</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>264.70100000000002</c:v>
+                  <c:v>266.72199999999998</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>268.65499999999997</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>270.50400000000002</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>272.27800000000002</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>273.98099999999999</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>275.625</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>277.20699999999999</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>278.738</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>280.21899999999999</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>281.654</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>283.048</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>284.399</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1501,7 +1789,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2743,13 +3031,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>19842</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>15874</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>488949</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>12699</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2779,13 +3067,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>379712</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>64447</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>198802</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>62751</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2814,10 +3102,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3137,10 +3421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48D945A2-F24A-4AFD-BFC7-713D375D8A61}">
-  <dimension ref="B3:F34"/>
+  <dimension ref="B3:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="65" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" zoomScale="54" zoomScaleNormal="65" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3162,416 +3446,651 @@
         <v>4</v>
       </c>
     </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B4">
+        <v>250</v>
+      </c>
+      <c r="C4">
+        <v>7266</v>
+      </c>
+      <c r="D4" s="1">
+        <v>186.37</v>
+      </c>
+      <c r="E4">
+        <v>7275</v>
+      </c>
+      <c r="F4">
+        <v>199.88499999999999</v>
+      </c>
+    </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B5">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="C5">
-        <v>7266</v>
-      </c>
-      <c r="D5" s="1">
-        <v>186.37</v>
+        <v>8723</v>
+      </c>
+      <c r="D5">
+        <v>191.68199999999999</v>
       </c>
       <c r="E5">
-        <v>7275</v>
+        <v>8736</v>
       </c>
       <c r="F5">
-        <v>199.88499999999999</v>
+        <v>205.21299999999999</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B6">
-        <v>300</v>
+        <v>350</v>
       </c>
       <c r="C6">
-        <v>8723</v>
+        <v>10180</v>
       </c>
       <c r="D6">
-        <v>191.68199999999999</v>
+        <v>196.173</v>
       </c>
       <c r="E6">
-        <v>8736</v>
+        <v>10213</v>
       </c>
       <c r="F6">
-        <v>205.21299999999999</v>
+        <v>209.76499999999999</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B7">
-        <v>350</v>
+        <v>400</v>
       </c>
       <c r="C7">
-        <v>10180</v>
+        <v>11640</v>
       </c>
       <c r="D7">
-        <v>196.173</v>
+        <v>200.071</v>
       </c>
       <c r="E7">
-        <v>10213</v>
+        <v>11711</v>
       </c>
       <c r="F7">
-        <v>209.76499999999999</v>
+        <v>213.76499999999999</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B8">
-        <v>400</v>
+        <v>450</v>
       </c>
       <c r="C8">
-        <v>11640</v>
+        <v>13105</v>
       </c>
       <c r="D8">
-        <v>200.071</v>
+        <v>203.523</v>
       </c>
       <c r="E8">
-        <v>11711</v>
+        <v>13228</v>
       </c>
       <c r="F8">
-        <v>213.76499999999999</v>
+        <v>217.34200000000001</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B9">
-        <v>450</v>
+        <v>500</v>
       </c>
       <c r="C9">
-        <v>13105</v>
-      </c>
-      <c r="D9">
-        <v>203.523</v>
+        <v>14581</v>
+      </c>
+      <c r="D9" s="1">
+        <v>206.63</v>
       </c>
       <c r="E9">
-        <v>13228</v>
+        <v>14770</v>
       </c>
       <c r="F9">
-        <v>217.34200000000001</v>
+        <v>220.589</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B10">
-        <v>500</v>
+        <v>550</v>
       </c>
       <c r="C10">
-        <v>14581</v>
-      </c>
-      <c r="D10" s="1">
-        <v>206.63</v>
+        <v>16064</v>
+      </c>
+      <c r="D10">
+        <v>209.46100000000001</v>
       </c>
       <c r="E10">
-        <v>14770</v>
+        <v>16338</v>
       </c>
       <c r="F10">
-        <v>220.589</v>
+        <v>223.57599999999999</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B11">
-        <v>550</v>
+        <v>600</v>
       </c>
       <c r="C11">
-        <v>16064</v>
+        <v>17563</v>
       </c>
       <c r="D11">
-        <v>209.46100000000001</v>
+        <v>212.066</v>
       </c>
       <c r="E11">
-        <v>16338</v>
+        <v>17929</v>
       </c>
       <c r="F11">
-        <v>223.57599999999999</v>
+        <v>226.346</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B12">
-        <v>600</v>
+        <v>650</v>
       </c>
       <c r="C12">
-        <v>17563</v>
+        <v>19075</v>
       </c>
       <c r="D12">
-        <v>212.066</v>
+        <v>214.489</v>
       </c>
       <c r="E12">
-        <v>17929</v>
+        <v>19544</v>
       </c>
       <c r="F12">
-        <v>226.346</v>
+        <v>228.93199999999999</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B13">
-        <v>650</v>
+        <v>700</v>
       </c>
       <c r="C13">
-        <v>19075</v>
+        <v>20604</v>
       </c>
       <c r="D13">
-        <v>214.489</v>
+        <v>216.756</v>
       </c>
       <c r="E13">
-        <v>19544</v>
+        <v>21184</v>
       </c>
       <c r="F13">
-        <v>228.93199999999999</v>
+        <v>231.358</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B14">
-        <v>700</v>
+        <v>750</v>
       </c>
       <c r="C14">
-        <v>20604</v>
+        <v>22149</v>
       </c>
       <c r="D14">
-        <v>216.756</v>
+        <v>218.88900000000001</v>
       </c>
       <c r="E14">
-        <v>21184</v>
+        <v>22844</v>
       </c>
       <c r="F14">
-        <v>231.358</v>
+        <v>233.649</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B15">
-        <v>750</v>
+        <v>800</v>
       </c>
       <c r="C15">
-        <v>22149</v>
+        <v>23714</v>
       </c>
       <c r="D15">
-        <v>218.88900000000001</v>
+        <v>220.90700000000001</v>
       </c>
       <c r="E15">
-        <v>22844</v>
-      </c>
-      <c r="F15">
-        <v>233.649</v>
+        <v>24523</v>
+      </c>
+      <c r="F15" s="1">
+        <v>235.81</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B16">
-        <v>800</v>
+        <v>850</v>
       </c>
       <c r="C16">
-        <v>23714</v>
+        <v>25292</v>
       </c>
       <c r="D16">
-        <v>220.90700000000001</v>
+        <v>222.822</v>
       </c>
       <c r="E16">
-        <v>24523</v>
-      </c>
-      <c r="F16" s="1">
-        <v>235.81</v>
+        <v>26218</v>
+      </c>
+      <c r="F16">
+        <v>237.864</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B17">
-        <v>850</v>
+        <v>900</v>
       </c>
       <c r="C17">
-        <v>25292</v>
+        <v>26890</v>
       </c>
       <c r="D17">
-        <v>222.822</v>
+        <v>224.64699999999999</v>
       </c>
       <c r="E17">
-        <v>26218</v>
+        <v>27928</v>
       </c>
       <c r="F17">
-        <v>237.864</v>
+        <v>239.82300000000001</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B18">
-        <v>900</v>
+        <v>950</v>
       </c>
       <c r="C18">
-        <v>26890</v>
+        <v>28501</v>
       </c>
       <c r="D18">
-        <v>224.64699999999999</v>
+        <v>226.38900000000001</v>
       </c>
       <c r="E18">
-        <v>27928</v>
+        <v>29652</v>
       </c>
       <c r="F18">
-        <v>239.82300000000001</v>
+        <v>241.68899999999999</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B19">
-        <v>950</v>
+        <v>1000</v>
       </c>
       <c r="C19">
-        <v>28501</v>
+        <v>30129</v>
       </c>
       <c r="D19">
-        <v>226.38900000000001</v>
+        <v>228.05699999999999</v>
       </c>
       <c r="E19">
-        <v>29652</v>
+        <v>31389</v>
       </c>
       <c r="F19">
-        <v>241.68899999999999</v>
+        <v>243.471</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B20">
-        <v>1000</v>
+        <v>1100</v>
       </c>
       <c r="C20">
-        <v>30129</v>
+        <v>33426</v>
       </c>
       <c r="D20">
-        <v>228.05699999999999</v>
+        <v>231.19900000000001</v>
       </c>
       <c r="E20">
-        <v>31389</v>
+        <v>34899</v>
       </c>
       <c r="F20">
-        <v>243.471</v>
+        <v>246.81800000000001</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B21">
-        <v>1100</v>
+        <v>1200</v>
       </c>
       <c r="C21">
-        <v>33426</v>
+        <v>36777</v>
       </c>
       <c r="D21">
-        <v>231.19900000000001</v>
+        <v>234.11500000000001</v>
       </c>
       <c r="E21">
-        <v>34899</v>
+        <v>38447</v>
       </c>
       <c r="F21">
-        <v>246.81800000000001</v>
+        <v>249.90600000000001</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B22">
-        <v>1200</v>
+        <v>1300</v>
       </c>
       <c r="C22">
-        <v>36777</v>
+        <v>40170</v>
       </c>
       <c r="D22">
-        <v>234.11500000000001</v>
+        <v>236.83099999999999</v>
       </c>
       <c r="E22">
-        <v>38447</v>
+        <v>42033</v>
       </c>
       <c r="F22">
-        <v>249.90600000000001</v>
+        <v>252.77600000000001</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B23">
-        <v>1300</v>
+        <v>1400</v>
       </c>
       <c r="C23">
-        <v>40170</v>
+        <v>43605</v>
       </c>
       <c r="D23">
-        <v>236.83099999999999</v>
+        <v>239.375</v>
       </c>
       <c r="E23">
-        <v>42033</v>
+        <v>45648</v>
       </c>
       <c r="F23">
-        <v>252.77600000000001</v>
+        <v>255.45400000000001</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B24">
-        <v>1400</v>
+        <v>1500</v>
       </c>
       <c r="C24">
-        <v>43605</v>
+        <v>47073</v>
       </c>
       <c r="D24">
-        <v>239.375</v>
+        <v>241.768</v>
       </c>
       <c r="E24">
-        <v>45648</v>
+        <v>49292</v>
       </c>
       <c r="F24">
-        <v>255.45400000000001</v>
+        <v>257.96499999999997</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B25">
-        <v>1500</v>
+        <v>1600</v>
       </c>
       <c r="C25">
-        <v>47073</v>
+        <v>50571</v>
       </c>
       <c r="D25">
-        <v>241.768</v>
+        <v>244.02799999999999</v>
       </c>
       <c r="E25">
-        <v>49292</v>
+        <v>52961</v>
       </c>
       <c r="F25">
-        <v>257.96499999999997</v>
+        <v>260.33300000000003</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B26">
-        <v>1600</v>
+        <v>1700</v>
       </c>
       <c r="C26">
-        <v>50571</v>
+        <v>54099</v>
       </c>
       <c r="D26">
-        <v>244.02799999999999</v>
+        <v>246.166</v>
       </c>
       <c r="E26">
-        <v>52961</v>
+        <v>56652</v>
       </c>
       <c r="F26">
-        <v>260.33300000000003</v>
+        <v>262.57100000000003</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B27">
-        <v>1700</v>
+        <v>1800</v>
       </c>
       <c r="C27">
-        <v>54099</v>
+        <v>57651</v>
       </c>
       <c r="D27">
-        <v>246.166</v>
+        <v>248.19499999999999</v>
       </c>
       <c r="E27">
-        <v>56652</v>
+        <v>60371</v>
       </c>
       <c r="F27">
-        <v>262.57100000000003</v>
+        <v>264.70100000000002</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B28">
-        <v>1800</v>
+        <v>1900</v>
       </c>
       <c r="C28">
-        <v>57651</v>
+        <v>61220</v>
       </c>
       <c r="D28">
-        <v>248.19499999999999</v>
+        <v>250.12799999999999</v>
       </c>
       <c r="E28">
-        <v>60371</v>
+        <v>64116</v>
       </c>
       <c r="F28">
-        <v>264.70100000000002</v>
+        <v>266.72199999999998</v>
       </c>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.45">
-      <c r="D34" s="1"/>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B29">
+        <v>2000</v>
+      </c>
+      <c r="C29">
+        <v>64810</v>
+      </c>
+      <c r="D29">
+        <v>251.96899999999999</v>
+      </c>
+      <c r="E29">
+        <v>67881</v>
+      </c>
+      <c r="F29">
+        <v>268.65499999999997</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B30">
+        <v>2100</v>
+      </c>
+      <c r="C30">
+        <v>68417</v>
+      </c>
+      <c r="D30">
+        <v>253.726</v>
+      </c>
+      <c r="E30">
+        <v>71668</v>
+      </c>
+      <c r="F30">
+        <v>270.50400000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B31">
+        <v>2200</v>
+      </c>
+      <c r="C31">
+        <v>72040</v>
+      </c>
+      <c r="D31">
+        <v>255.41200000000001</v>
+      </c>
+      <c r="E31">
+        <v>75484</v>
+      </c>
+      <c r="F31">
+        <v>272.27800000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B32">
+        <v>2300</v>
+      </c>
+      <c r="C32">
+        <v>75676</v>
+      </c>
+      <c r="D32">
+        <v>257.02699999999999</v>
+      </c>
+      <c r="E32">
+        <v>79316</v>
+      </c>
+      <c r="F32">
+        <v>273.98099999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B33">
+        <v>2400</v>
+      </c>
+      <c r="C33">
+        <v>79320</v>
+      </c>
+      <c r="D33" s="1">
+        <v>258.58</v>
+      </c>
+      <c r="E33">
+        <v>83174</v>
+      </c>
+      <c r="F33">
+        <v>275.625</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B34">
+        <v>2500</v>
+      </c>
+      <c r="C34">
+        <v>82981</v>
+      </c>
+      <c r="D34">
+        <v>260.07299999999998</v>
+      </c>
+      <c r="E34">
+        <v>87057</v>
+      </c>
+      <c r="F34">
+        <v>277.20699999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B35">
+        <v>2600</v>
+      </c>
+      <c r="C35">
+        <v>86650</v>
+      </c>
+      <c r="D35">
+        <v>261.512</v>
+      </c>
+      <c r="E35">
+        <v>90956</v>
+      </c>
+      <c r="F35">
+        <v>278.738</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B36">
+        <v>2700</v>
+      </c>
+      <c r="C36">
+        <v>90328</v>
+      </c>
+      <c r="D36">
+        <v>262.90199999999999</v>
+      </c>
+      <c r="E36">
+        <v>94881</v>
+      </c>
+      <c r="F36">
+        <v>280.21899999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B37">
+        <v>2800</v>
+      </c>
+      <c r="C37">
+        <v>94014</v>
+      </c>
+      <c r="D37">
+        <v>264.24099999999999</v>
+      </c>
+      <c r="E37">
+        <v>98826</v>
+      </c>
+      <c r="F37">
+        <v>281.654</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B38">
+        <v>2900</v>
+      </c>
+      <c r="C38">
+        <v>97705</v>
+      </c>
+      <c r="D38">
+        <v>265.53800000000001</v>
+      </c>
+      <c r="E38">
+        <v>102793</v>
+      </c>
+      <c r="F38">
+        <v>283.048</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B39">
+        <v>3000</v>
+      </c>
+      <c r="C39">
+        <v>101407</v>
+      </c>
+      <c r="D39">
+        <v>266.79300000000001</v>
+      </c>
+      <c r="E39">
+        <v>106780</v>
+      </c>
+      <c r="F39">
+        <v>284.399</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B40">
+        <v>3100</v>
+      </c>
+      <c r="C40">
+        <v>105115</v>
+      </c>
+      <c r="D40">
+        <v>268.00700000000001</v>
+      </c>
+      <c r="E40">
+        <v>110784</v>
+      </c>
+      <c r="F40">
+        <v>285.71300000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B41">
+        <v>3200</v>
+      </c>
+      <c r="C41">
+        <v>108830</v>
+      </c>
+      <c r="D41">
+        <v>269.18599999999998</v>
+      </c>
+      <c r="E41">
+        <v>114809</v>
+      </c>
+      <c r="F41">
+        <v>286.98899999999998</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3580,12 +4099,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="7f3ca868-b031-4e60-87f4-a1bfe4f2ec3c" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3785,17 +4303,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="7f3ca868-b031-4e60-87f4-a1bfe4f2ec3c" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E00589F-6A95-404C-9940-B281A1AB26E9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{796A5BBF-1CA1-4B58-BB05-F028BCC8BF96}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7f3ca868-b031-4e60-87f4-a1bfe4f2ec3c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3819,17 +4346,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{796A5BBF-1CA1-4B58-BB05-F028BCC8BF96}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E00589F-6A95-404C-9940-B281A1AB26E9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7f3ca868-b031-4e60-87f4-a1bfe4f2ec3c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
i dont know whats going on
</commit_message>
<xml_diff>
--- a/polynomial calcs.xlsx
+++ b/polynomial calcs.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\embas\Documents\GitHub\Thermal-Fluids-Gas-Turbine-Simulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{486E814F-4F20-424F-8D6A-B748ED6D57E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2723CCF6-0C60-4452-975A-C5C89079310A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{7ECF82CD-4B31-4C5B-B4C1-F49AFA1B0555}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028" concurrentCalc="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -57,9 +57,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.000"/>
-  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -89,9 +86,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -227,112 +223,112 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="36"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>250</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="5">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>298</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>300</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="11">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>350</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="16">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>400</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="21">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>430</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>450</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="26">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>470</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>490</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>500</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="31">
+                  <c:v>510</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>520</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>540</c:v>
+                </c:pt>
+                <c:pt idx="35">
                   <c:v>550</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>600</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>650</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>700</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>750</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>800</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>850</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>900</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>950</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1100</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1200</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1300</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1400</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1500</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1600</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1700</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1800</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1900</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>2100</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>2200</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>2300</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>2400</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>2500</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>2600</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>2700</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>2800</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>2900</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>3000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -344,112 +340,112 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="36"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6391</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6683</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6975</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>7266</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="5">
+                  <c:v>7558</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7849</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8141</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8432</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8669</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>8723</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="11">
+                  <c:v>9014</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9306</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9597</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9888</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>10180</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="16">
+                  <c:v>10471</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>10763</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11055</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>11347</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>11640</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="21">
+                  <c:v>11932</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>12225</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>12518</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12811</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>13105</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="26">
+                  <c:v>13399</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>13693</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>13988</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>14285</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>14581</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="31">
+                  <c:v>14876</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>15172</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>15469</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>15766</c:v>
+                </c:pt>
+                <c:pt idx="35">
                   <c:v>16064</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>17563</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>19075</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>20604</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>22149</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>23714</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>25292</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>26890</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>28501</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>30129</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>33426</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>36777</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>40170</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>43605</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>47073</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>50571</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>54099</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>57651</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>61220</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>64810</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>68417</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>72040</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>75676</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>79320</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>82981</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>86650</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>90328</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>94014</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>97705</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>101407</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -559,112 +555,112 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="36"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>250</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="5">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>298</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>300</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="11">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>350</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="16">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>400</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="21">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>430</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>450</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="26">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>470</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>490</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>500</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="31">
+                  <c:v>510</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>520</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>540</c:v>
+                </c:pt>
+                <c:pt idx="35">
                   <c:v>550</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>600</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>650</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>700</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>750</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>800</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>850</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>900</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>950</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1100</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1200</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1300</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1400</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1500</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1600</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1700</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1800</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1900</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>2100</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>2200</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>2300</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>2400</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>2500</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>2600</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>2700</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>2800</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>2900</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>3000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -676,112 +672,112 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="36"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6404</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6694</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6984</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>7275</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="5">
+                  <c:v>7566</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7858</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8150</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8443</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8682</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>8736</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="11">
+                  <c:v>9030</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9325</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9620</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9916</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>10213</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="16">
+                  <c:v>10511</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>10809</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11109</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>11409</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>11711</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="21">
+                  <c:v>12012</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>12314</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>12618</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12923</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>13228</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="26">
+                  <c:v>13535</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>13842</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>14151</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>14460</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>14770</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="31">
+                  <c:v>15082</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>15395</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>15708</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>16022</c:v>
+                </c:pt>
+                <c:pt idx="35">
                   <c:v>16338</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>17929</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>19544</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>21184</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>22844</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>24523</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>26218</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>27928</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>29652</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>31389</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>34899</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>38447</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>42033</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>45648</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>49292</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>52961</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>56652</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>60371</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>64116</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>67881</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>71668</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>75484</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>79316</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>83174</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>87057</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>90956</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>94881</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>98826</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>102793</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>106780</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1129,112 +1125,112 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="36"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>250</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="5">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>298</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>300</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="11">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>350</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="16">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>400</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="21">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>430</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>450</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="26">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>470</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>490</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>500</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="31">
+                  <c:v>510</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>520</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>540</c:v>
+                </c:pt>
+                <c:pt idx="35">
                   <c:v>550</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>600</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>650</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>700</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>750</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>800</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>850</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>900</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>950</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1100</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1200</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1300</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1400</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1500</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1600</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1700</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1800</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1900</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>2100</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>2200</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>2300</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>2400</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>2500</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>2600</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>2700</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>2800</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>2900</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>3000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1245,113 +1241,113 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="36"/>
-                <c:pt idx="0" formatCode="0.000">
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>182.63800000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>183.93799999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>185.18</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>186.37</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="5">
+                  <c:v>187.51400000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>188.614</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>189.673</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>190.69499999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>191.50200000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>191.68199999999999</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="11">
+                  <c:v>192.63800000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>193.56200000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>194.459</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>195.328</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>196.173</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="16">
+                  <c:v>196.995</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>197.79400000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>198.572</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>199.33099999999999</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>200.071</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="21">
+                  <c:v>200.79400000000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>201.499</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>202.18899999999999</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>202.863</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>203.523</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="0.000">
+                <c:pt idx="26">
+                  <c:v>204.17</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>204.803</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>205.42400000000001</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>206.03299999999999</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>206.63</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="31">
+                  <c:v>207.21600000000001</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>207.792</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>208.358</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>208.91399999999999</c:v>
+                </c:pt>
+                <c:pt idx="35">
                   <c:v>209.46100000000001</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>212.066</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>214.489</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>216.756</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>218.88900000000001</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>220.90700000000001</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>222.822</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>224.64699999999999</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>226.38900000000001</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>228.05699999999999</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>231.19900000000001</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>234.11500000000001</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>236.83099999999999</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>239.375</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>241.768</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>244.02799999999999</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>246.166</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>248.19499999999999</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>250.12799999999999</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>251.96899999999999</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>253.726</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>255.41200000000001</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>257.02699999999999</c:v>
-                </c:pt>
-                <c:pt idx="29" formatCode="0.000">
-                  <c:v>258.58</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>260.07299999999998</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>261.512</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>262.90199999999999</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>264.24099999999999</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>265.53800000000001</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>266.79300000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1461,112 +1457,112 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="36"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>250</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="5">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>298</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>300</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="11">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>350</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="16">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>400</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="21">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>430</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>450</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="26">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>470</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>490</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>500</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="31">
+                  <c:v>510</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>520</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>540</c:v>
+                </c:pt>
+                <c:pt idx="35">
                   <c:v>550</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>600</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>650</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>700</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>750</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>800</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>850</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>900</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>950</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1100</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1200</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1300</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1400</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1500</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1600</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1700</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1800</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1900</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>2100</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>2200</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>2300</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>2400</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>2500</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>2600</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>2700</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>2800</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>2900</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>3000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1578,112 +1574,112 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="36"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>196.17099999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>197.46100000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>198.696</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>199.88499999999999</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="5">
+                  <c:v>201.02699999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>202.12799999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>203.191</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>204.21799999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>205.03299999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>205.21299999999999</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="11">
+                  <c:v>206.17699999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>207.11199999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>208.02</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>208.904</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>209.76499999999999</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="16">
+                  <c:v>210.60400000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>211.423</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>212.22200000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>213.00200000000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>213.76499999999999</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="21">
+                  <c:v>214.51</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>215.24100000000001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>215.95500000000001</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>216.65600000000001</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>217.34200000000001</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="26">
+                  <c:v>218.01599999999999</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>218.67599999999999</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>219.32599999999999</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>219.96299999999999</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>220.589</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="31">
+                  <c:v>221.20599999999999</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>221.81200000000001</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>222.40899999999999</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>222.99700000000001</c:v>
+                </c:pt>
+                <c:pt idx="35">
                   <c:v>223.57599999999999</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>226.346</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>228.93199999999999</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>231.358</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>233.649</c:v>
-                </c:pt>
-                <c:pt idx="11" formatCode="0.000">
-                  <c:v>235.81</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>237.864</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>239.82300000000001</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>241.68899999999999</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>243.471</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>246.81800000000001</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>249.90600000000001</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>252.77600000000001</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>255.45400000000001</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>257.96499999999997</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>260.33300000000003</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>262.57100000000003</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>264.70100000000002</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>266.72199999999998</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>268.65499999999997</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>270.50400000000002</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>272.27800000000002</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>273.98099999999999</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>275.625</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>277.20699999999999</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>278.738</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>280.21899999999999</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>281.654</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>283.048</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>284.399</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1789,7 +1785,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3421,10 +3417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48D945A2-F24A-4AFD-BFC7-713D375D8A61}">
-  <dimension ref="B3:F41"/>
+  <dimension ref="B3:F159"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="54" zoomScaleNormal="65" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="70" zoomScaleNormal="65" workbookViewId="0">
+      <selection activeCell="U45" sqref="U45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3448,648 +3444,2654 @@
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B4">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>7266</v>
-      </c>
-      <c r="D4" s="1">
-        <v>186.37</v>
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>7275</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>199.88499999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B5">
-        <v>300</v>
+        <v>220</v>
       </c>
       <c r="C5">
-        <v>8723</v>
+        <v>6391</v>
       </c>
       <c r="D5">
-        <v>191.68199999999999</v>
+        <v>182.63800000000001</v>
       </c>
       <c r="E5">
-        <v>8736</v>
+        <v>6404</v>
       </c>
       <c r="F5">
-        <v>205.21299999999999</v>
+        <v>196.17099999999999</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B6">
-        <v>350</v>
+        <v>230</v>
       </c>
       <c r="C6">
-        <v>10180</v>
+        <v>6683</v>
       </c>
       <c r="D6">
-        <v>196.173</v>
+        <v>183.93799999999999</v>
       </c>
       <c r="E6">
-        <v>10213</v>
+        <v>6694</v>
       </c>
       <c r="F6">
-        <v>209.76499999999999</v>
+        <v>197.46100000000001</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B7">
-        <v>400</v>
+        <v>240</v>
       </c>
       <c r="C7">
-        <v>11640</v>
+        <v>6975</v>
       </c>
       <c r="D7">
-        <v>200.071</v>
+        <v>185.18</v>
       </c>
       <c r="E7">
-        <v>11711</v>
+        <v>6984</v>
       </c>
       <c r="F7">
-        <v>213.76499999999999</v>
+        <v>198.696</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B8">
-        <v>450</v>
+        <v>250</v>
       </c>
       <c r="C8">
-        <v>13105</v>
+        <v>7266</v>
       </c>
       <c r="D8">
-        <v>203.523</v>
+        <v>186.37</v>
       </c>
       <c r="E8">
-        <v>13228</v>
+        <v>7275</v>
       </c>
       <c r="F8">
-        <v>217.34200000000001</v>
+        <v>199.88499999999999</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B9">
-        <v>500</v>
+        <v>260</v>
       </c>
       <c r="C9">
-        <v>14581</v>
-      </c>
-      <c r="D9" s="1">
-        <v>206.63</v>
+        <v>7558</v>
+      </c>
+      <c r="D9">
+        <v>187.51400000000001</v>
       </c>
       <c r="E9">
-        <v>14770</v>
+        <v>7566</v>
       </c>
       <c r="F9">
-        <v>220.589</v>
+        <v>201.02699999999999</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B10">
-        <v>550</v>
+        <v>270</v>
       </c>
       <c r="C10">
-        <v>16064</v>
+        <v>7849</v>
       </c>
       <c r="D10">
-        <v>209.46100000000001</v>
+        <v>188.614</v>
       </c>
       <c r="E10">
-        <v>16338</v>
+        <v>7858</v>
       </c>
       <c r="F10">
-        <v>223.57599999999999</v>
+        <v>202.12799999999999</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B11">
-        <v>600</v>
+        <v>280</v>
       </c>
       <c r="C11">
-        <v>17563</v>
+        <v>8141</v>
       </c>
       <c r="D11">
-        <v>212.066</v>
+        <v>189.673</v>
       </c>
       <c r="E11">
-        <v>17929</v>
+        <v>8150</v>
       </c>
       <c r="F11">
-        <v>226.346</v>
+        <v>203.191</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B12">
-        <v>650</v>
+        <v>290</v>
       </c>
       <c r="C12">
-        <v>19075</v>
+        <v>8432</v>
       </c>
       <c r="D12">
-        <v>214.489</v>
+        <v>190.69499999999999</v>
       </c>
       <c r="E12">
-        <v>19544</v>
+        <v>8443</v>
       </c>
       <c r="F12">
-        <v>228.93199999999999</v>
+        <v>204.21799999999999</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B13">
-        <v>700</v>
+        <v>298</v>
       </c>
       <c r="C13">
-        <v>20604</v>
+        <v>8669</v>
       </c>
       <c r="D13">
-        <v>216.756</v>
+        <v>191.50200000000001</v>
       </c>
       <c r="E13">
-        <v>21184</v>
+        <v>8682</v>
       </c>
       <c r="F13">
-        <v>231.358</v>
+        <v>205.03299999999999</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B14">
-        <v>750</v>
+        <v>300</v>
       </c>
       <c r="C14">
-        <v>22149</v>
+        <v>8723</v>
       </c>
       <c r="D14">
-        <v>218.88900000000001</v>
+        <v>191.68199999999999</v>
       </c>
       <c r="E14">
-        <v>22844</v>
+        <v>8736</v>
       </c>
       <c r="F14">
-        <v>233.649</v>
+        <v>205.21299999999999</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B15">
-        <v>800</v>
+        <v>310</v>
       </c>
       <c r="C15">
-        <v>23714</v>
+        <v>9014</v>
       </c>
       <c r="D15">
-        <v>220.90700000000001</v>
+        <v>192.63800000000001</v>
       </c>
       <c r="E15">
-        <v>24523</v>
-      </c>
-      <c r="F15" s="1">
-        <v>235.81</v>
+        <v>9030</v>
+      </c>
+      <c r="F15">
+        <v>206.17699999999999</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B16">
-        <v>850</v>
+        <v>320</v>
       </c>
       <c r="C16">
-        <v>25292</v>
+        <v>9306</v>
       </c>
       <c r="D16">
-        <v>222.822</v>
+        <v>193.56200000000001</v>
       </c>
       <c r="E16">
-        <v>26218</v>
+        <v>9325</v>
       </c>
       <c r="F16">
-        <v>237.864</v>
+        <v>207.11199999999999</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B17">
-        <v>900</v>
+        <v>330</v>
       </c>
       <c r="C17">
-        <v>26890</v>
+        <v>9597</v>
       </c>
       <c r="D17">
-        <v>224.64699999999999</v>
+        <v>194.459</v>
       </c>
       <c r="E17">
-        <v>27928</v>
+        <v>9620</v>
       </c>
       <c r="F17">
-        <v>239.82300000000001</v>
+        <v>208.02</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B18">
-        <v>950</v>
+        <v>340</v>
       </c>
       <c r="C18">
-        <v>28501</v>
+        <v>9888</v>
       </c>
       <c r="D18">
-        <v>226.38900000000001</v>
+        <v>195.328</v>
       </c>
       <c r="E18">
-        <v>29652</v>
+        <v>9916</v>
       </c>
       <c r="F18">
-        <v>241.68899999999999</v>
+        <v>208.904</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B19">
-        <v>1000</v>
+        <v>350</v>
       </c>
       <c r="C19">
-        <v>30129</v>
+        <v>10180</v>
       </c>
       <c r="D19">
-        <v>228.05699999999999</v>
+        <v>196.173</v>
       </c>
       <c r="E19">
-        <v>31389</v>
+        <v>10213</v>
       </c>
       <c r="F19">
-        <v>243.471</v>
+        <v>209.76499999999999</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B20">
-        <v>1100</v>
+        <v>360</v>
       </c>
       <c r="C20">
-        <v>33426</v>
+        <v>10471</v>
       </c>
       <c r="D20">
-        <v>231.19900000000001</v>
+        <v>196.995</v>
       </c>
       <c r="E20">
-        <v>34899</v>
+        <v>10511</v>
       </c>
       <c r="F20">
-        <v>246.81800000000001</v>
+        <v>210.60400000000001</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B21">
-        <v>1200</v>
+        <v>370</v>
       </c>
       <c r="C21">
-        <v>36777</v>
+        <v>10763</v>
       </c>
       <c r="D21">
-        <v>234.11500000000001</v>
+        <v>197.79400000000001</v>
       </c>
       <c r="E21">
-        <v>38447</v>
+        <v>10809</v>
       </c>
       <c r="F21">
-        <v>249.90600000000001</v>
+        <v>211.423</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B22">
-        <v>1300</v>
+        <v>380</v>
       </c>
       <c r="C22">
-        <v>40170</v>
+        <v>11055</v>
       </c>
       <c r="D22">
-        <v>236.83099999999999</v>
+        <v>198.572</v>
       </c>
       <c r="E22">
-        <v>42033</v>
+        <v>11109</v>
       </c>
       <c r="F22">
-        <v>252.77600000000001</v>
+        <v>212.22200000000001</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B23">
-        <v>1400</v>
+        <v>390</v>
       </c>
       <c r="C23">
-        <v>43605</v>
+        <v>11347</v>
       </c>
       <c r="D23">
-        <v>239.375</v>
+        <v>199.33099999999999</v>
       </c>
       <c r="E23">
-        <v>45648</v>
+        <v>11409</v>
       </c>
       <c r="F23">
-        <v>255.45400000000001</v>
+        <v>213.00200000000001</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B24">
-        <v>1500</v>
+        <v>400</v>
       </c>
       <c r="C24">
-        <v>47073</v>
+        <v>11640</v>
       </c>
       <c r="D24">
-        <v>241.768</v>
+        <v>200.071</v>
       </c>
       <c r="E24">
-        <v>49292</v>
+        <v>11711</v>
       </c>
       <c r="F24">
-        <v>257.96499999999997</v>
+        <v>213.76499999999999</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B25">
-        <v>1600</v>
+        <v>410</v>
       </c>
       <c r="C25">
-        <v>50571</v>
+        <v>11932</v>
       </c>
       <c r="D25">
-        <v>244.02799999999999</v>
+        <v>200.79400000000001</v>
       </c>
       <c r="E25">
-        <v>52961</v>
+        <v>12012</v>
       </c>
       <c r="F25">
-        <v>260.33300000000003</v>
+        <v>214.51</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B26">
-        <v>1700</v>
+        <v>420</v>
       </c>
       <c r="C26">
-        <v>54099</v>
+        <v>12225</v>
       </c>
       <c r="D26">
-        <v>246.166</v>
+        <v>201.499</v>
       </c>
       <c r="E26">
-        <v>56652</v>
+        <v>12314</v>
       </c>
       <c r="F26">
-        <v>262.57100000000003</v>
+        <v>215.24100000000001</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B27">
-        <v>1800</v>
+        <v>430</v>
       </c>
       <c r="C27">
-        <v>57651</v>
+        <v>12518</v>
       </c>
       <c r="D27">
-        <v>248.19499999999999</v>
+        <v>202.18899999999999</v>
       </c>
       <c r="E27">
-        <v>60371</v>
+        <v>12618</v>
       </c>
       <c r="F27">
-        <v>264.70100000000002</v>
+        <v>215.95500000000001</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B28">
-        <v>1900</v>
+        <v>440</v>
       </c>
       <c r="C28">
-        <v>61220</v>
+        <v>12811</v>
       </c>
       <c r="D28">
-        <v>250.12799999999999</v>
+        <v>202.863</v>
       </c>
       <c r="E28">
-        <v>64116</v>
+        <v>12923</v>
       </c>
       <c r="F28">
-        <v>266.72199999999998</v>
+        <v>216.65600000000001</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B29">
-        <v>2000</v>
+        <v>450</v>
       </c>
       <c r="C29">
-        <v>64810</v>
+        <v>13105</v>
       </c>
       <c r="D29">
-        <v>251.96899999999999</v>
+        <v>203.523</v>
       </c>
       <c r="E29">
-        <v>67881</v>
+        <v>13228</v>
       </c>
       <c r="F29">
-        <v>268.65499999999997</v>
+        <v>217.34200000000001</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B30">
-        <v>2100</v>
+        <v>460</v>
       </c>
       <c r="C30">
-        <v>68417</v>
+        <v>13399</v>
       </c>
       <c r="D30">
-        <v>253.726</v>
+        <v>204.17</v>
       </c>
       <c r="E30">
-        <v>71668</v>
+        <v>13535</v>
       </c>
       <c r="F30">
-        <v>270.50400000000002</v>
+        <v>218.01599999999999</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B31">
-        <v>2200</v>
+        <v>470</v>
       </c>
       <c r="C31">
-        <v>72040</v>
+        <v>13693</v>
       </c>
       <c r="D31">
-        <v>255.41200000000001</v>
+        <v>204.803</v>
       </c>
       <c r="E31">
-        <v>75484</v>
+        <v>13842</v>
       </c>
       <c r="F31">
-        <v>272.27800000000002</v>
+        <v>218.67599999999999</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B32">
-        <v>2300</v>
+        <v>480</v>
       </c>
       <c r="C32">
-        <v>75676</v>
+        <v>13988</v>
       </c>
       <c r="D32">
-        <v>257.02699999999999</v>
+        <v>205.42400000000001</v>
       </c>
       <c r="E32">
-        <v>79316</v>
+        <v>14151</v>
       </c>
       <c r="F32">
-        <v>273.98099999999999</v>
+        <v>219.32599999999999</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B33">
-        <v>2400</v>
+        <v>490</v>
       </c>
       <c r="C33">
-        <v>79320</v>
-      </c>
-      <c r="D33" s="1">
-        <v>258.58</v>
+        <v>14285</v>
+      </c>
+      <c r="D33">
+        <v>206.03299999999999</v>
       </c>
       <c r="E33">
-        <v>83174</v>
+        <v>14460</v>
       </c>
       <c r="F33">
-        <v>275.625</v>
+        <v>219.96299999999999</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B34">
-        <v>2500</v>
+        <v>500</v>
       </c>
       <c r="C34">
-        <v>82981</v>
+        <v>14581</v>
       </c>
       <c r="D34">
-        <v>260.07299999999998</v>
+        <v>206.63</v>
       </c>
       <c r="E34">
-        <v>87057</v>
+        <v>14770</v>
       </c>
       <c r="F34">
-        <v>277.20699999999999</v>
+        <v>220.589</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B35">
-        <v>2600</v>
+        <v>510</v>
       </c>
       <c r="C35">
-        <v>86650</v>
+        <v>14876</v>
       </c>
       <c r="D35">
-        <v>261.512</v>
+        <v>207.21600000000001</v>
       </c>
       <c r="E35">
-        <v>90956</v>
+        <v>15082</v>
       </c>
       <c r="F35">
-        <v>278.738</v>
+        <v>221.20599999999999</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B36">
-        <v>2700</v>
+        <v>520</v>
       </c>
       <c r="C36">
-        <v>90328</v>
+        <v>15172</v>
       </c>
       <c r="D36">
-        <v>262.90199999999999</v>
+        <v>207.792</v>
       </c>
       <c r="E36">
-        <v>94881</v>
+        <v>15395</v>
       </c>
       <c r="F36">
-        <v>280.21899999999999</v>
+        <v>221.81200000000001</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B37">
-        <v>2800</v>
+        <v>530</v>
       </c>
       <c r="C37">
-        <v>94014</v>
+        <v>15469</v>
       </c>
       <c r="D37">
-        <v>264.24099999999999</v>
+        <v>208.358</v>
       </c>
       <c r="E37">
-        <v>98826</v>
+        <v>15708</v>
       </c>
       <c r="F37">
-        <v>281.654</v>
+        <v>222.40899999999999</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B38">
-        <v>2900</v>
+        <v>540</v>
       </c>
       <c r="C38">
-        <v>97705</v>
+        <v>15766</v>
       </c>
       <c r="D38">
-        <v>265.53800000000001</v>
+        <v>208.91399999999999</v>
       </c>
       <c r="E38">
-        <v>102793</v>
+        <v>16022</v>
       </c>
       <c r="F38">
-        <v>283.048</v>
+        <v>222.99700000000001</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B39">
-        <v>3000</v>
+        <v>550</v>
       </c>
       <c r="C39">
-        <v>101407</v>
+        <v>16064</v>
       </c>
       <c r="D39">
-        <v>266.79300000000001</v>
+        <v>209.46100000000001</v>
       </c>
       <c r="E39">
-        <v>106780</v>
+        <v>16338</v>
       </c>
       <c r="F39">
-        <v>284.399</v>
+        <v>223.57599999999999</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B40">
-        <v>3100</v>
+        <v>560</v>
       </c>
       <c r="C40">
-        <v>105115</v>
+        <v>16363</v>
       </c>
       <c r="D40">
-        <v>268.00700000000001</v>
+        <v>209.999</v>
       </c>
       <c r="E40">
-        <v>110784</v>
+        <v>16654</v>
       </c>
       <c r="F40">
-        <v>285.71300000000002</v>
+        <v>224.14599999999999</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B41">
+        <v>570</v>
+      </c>
+      <c r="C41">
+        <v>16662</v>
+      </c>
+      <c r="D41">
+        <v>210.52799999999999</v>
+      </c>
+      <c r="E41">
+        <v>16971</v>
+      </c>
+      <c r="F41">
+        <v>224.708</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B42">
+        <v>580</v>
+      </c>
+      <c r="C42">
+        <v>16962</v>
+      </c>
+      <c r="D42">
+        <v>211.04900000000001</v>
+      </c>
+      <c r="E42">
+        <v>17290</v>
+      </c>
+      <c r="F42">
+        <v>225.262</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B43">
+        <v>590</v>
+      </c>
+      <c r="C43">
+        <v>17262</v>
+      </c>
+      <c r="D43">
+        <v>211.56200000000001</v>
+      </c>
+      <c r="E43">
+        <v>17609</v>
+      </c>
+      <c r="F43">
+        <v>225.80799999999999</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B44">
+        <v>600</v>
+      </c>
+      <c r="C44">
+        <v>17563</v>
+      </c>
+      <c r="D44">
+        <v>212.066</v>
+      </c>
+      <c r="E44">
+        <v>17929</v>
+      </c>
+      <c r="F44">
+        <v>226.346</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B45">
+        <v>610</v>
+      </c>
+      <c r="C45">
+        <v>17864</v>
+      </c>
+      <c r="D45">
+        <v>212.56399999999999</v>
+      </c>
+      <c r="E45">
+        <v>18250</v>
+      </c>
+      <c r="F45">
+        <v>226.87700000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B46">
+        <v>620</v>
+      </c>
+      <c r="C46">
+        <v>18166</v>
+      </c>
+      <c r="D46">
+        <v>213.05500000000001</v>
+      </c>
+      <c r="E46">
+        <v>18572</v>
+      </c>
+      <c r="F46">
+        <v>227.4</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B47">
+        <v>630</v>
+      </c>
+      <c r="C47">
+        <v>18468</v>
+      </c>
+      <c r="D47">
+        <v>213.541</v>
+      </c>
+      <c r="E47">
+        <v>18895</v>
+      </c>
+      <c r="F47">
+        <v>227.91800000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B48">
+        <v>640</v>
+      </c>
+      <c r="C48">
+        <v>18772</v>
+      </c>
+      <c r="D48">
+        <v>214.018</v>
+      </c>
+      <c r="E48">
+        <v>19219</v>
+      </c>
+      <c r="F48">
+        <v>228.429</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B49">
+        <v>650</v>
+      </c>
+      <c r="C49">
+        <v>19075</v>
+      </c>
+      <c r="D49">
+        <v>214.489</v>
+      </c>
+      <c r="E49">
+        <v>19544</v>
+      </c>
+      <c r="F49">
+        <v>228.93199999999999</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B50">
+        <v>660</v>
+      </c>
+      <c r="C50">
+        <v>19380</v>
+      </c>
+      <c r="D50">
+        <v>214.95400000000001</v>
+      </c>
+      <c r="E50">
+        <v>19870</v>
+      </c>
+      <c r="F50">
+        <v>229.43</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B51">
+        <v>670</v>
+      </c>
+      <c r="C51">
+        <v>19685</v>
+      </c>
+      <c r="D51">
+        <v>215.41300000000001</v>
+      </c>
+      <c r="E51">
+        <v>20197</v>
+      </c>
+      <c r="F51">
+        <v>229.92</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B52">
+        <v>680</v>
+      </c>
+      <c r="C52">
+        <v>19991</v>
+      </c>
+      <c r="D52">
+        <v>215.86600000000001</v>
+      </c>
+      <c r="E52">
+        <v>20524</v>
+      </c>
+      <c r="F52">
+        <v>230.405</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B53">
+        <v>690</v>
+      </c>
+      <c r="C53">
+        <v>20297</v>
+      </c>
+      <c r="D53">
+        <v>216.31399999999999</v>
+      </c>
+      <c r="E53">
+        <v>20854</v>
+      </c>
+      <c r="F53">
+        <v>230.88499999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B54">
+        <v>700</v>
+      </c>
+      <c r="C54">
+        <v>20604</v>
+      </c>
+      <c r="D54">
+        <v>216.756</v>
+      </c>
+      <c r="E54">
+        <v>21184</v>
+      </c>
+      <c r="F54">
+        <v>231.358</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B55">
+        <v>710</v>
+      </c>
+      <c r="C55">
+        <v>20912</v>
+      </c>
+      <c r="D55">
+        <v>217.19200000000001</v>
+      </c>
+      <c r="E55">
+        <v>21514</v>
+      </c>
+      <c r="F55">
+        <v>231.827</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B56">
+        <v>720</v>
+      </c>
+      <c r="C56">
+        <v>21220</v>
+      </c>
+      <c r="D56">
+        <v>217.624</v>
+      </c>
+      <c r="E56">
+        <v>21845</v>
+      </c>
+      <c r="F56">
+        <v>232.291</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B57">
+        <v>730</v>
+      </c>
+      <c r="C57">
+        <v>21529</v>
+      </c>
+      <c r="D57">
+        <v>218.059</v>
+      </c>
+      <c r="E57">
+        <v>22177</v>
+      </c>
+      <c r="F57">
+        <v>232.74799999999999</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B58">
+        <v>740</v>
+      </c>
+      <c r="C58">
+        <v>21839</v>
+      </c>
+      <c r="D58">
+        <v>218.47200000000001</v>
+      </c>
+      <c r="E58">
+        <v>22510</v>
+      </c>
+      <c r="F58">
+        <v>233.20099999999999</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B59">
+        <v>750</v>
+      </c>
+      <c r="C59">
+        <v>22149</v>
+      </c>
+      <c r="D59">
+        <v>218.88900000000001</v>
+      </c>
+      <c r="E59">
+        <v>22844</v>
+      </c>
+      <c r="F59">
+        <v>233.649</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B60">
+        <v>760</v>
+      </c>
+      <c r="C60">
+        <v>22460</v>
+      </c>
+      <c r="D60">
+        <v>219.30099999999999</v>
+      </c>
+      <c r="E60">
+        <v>23178</v>
+      </c>
+      <c r="F60">
+        <v>234.09100000000001</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B61">
+        <v>770</v>
+      </c>
+      <c r="C61">
+        <v>22772</v>
+      </c>
+      <c r="D61">
+        <v>219.709</v>
+      </c>
+      <c r="E61">
+        <v>23513</v>
+      </c>
+      <c r="F61">
+        <v>234.52799999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B62">
+        <v>780</v>
+      </c>
+      <c r="C62">
+        <v>23085</v>
+      </c>
+      <c r="D62">
+        <v>220.113</v>
+      </c>
+      <c r="E62">
+        <v>23850</v>
+      </c>
+      <c r="F62">
+        <v>234.96</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B63">
+        <v>790</v>
+      </c>
+      <c r="C63">
+        <v>23398</v>
+      </c>
+      <c r="D63">
+        <v>220.512</v>
+      </c>
+      <c r="E63">
+        <v>24186</v>
+      </c>
+      <c r="F63">
+        <v>235.387</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B64">
+        <v>800</v>
+      </c>
+      <c r="C64">
+        <v>23714</v>
+      </c>
+      <c r="D64">
+        <v>220.90700000000001</v>
+      </c>
+      <c r="E64">
+        <v>24523</v>
+      </c>
+      <c r="F64">
+        <v>235.81</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B65">
+        <v>810</v>
+      </c>
+      <c r="C65">
+        <v>24027</v>
+      </c>
+      <c r="D65">
+        <v>221.298</v>
+      </c>
+      <c r="E65">
+        <v>24861</v>
+      </c>
+      <c r="F65">
+        <v>236.23</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B66">
+        <v>820</v>
+      </c>
+      <c r="C66">
+        <v>24342</v>
+      </c>
+      <c r="D66">
+        <v>221.684</v>
+      </c>
+      <c r="E66">
+        <v>25199</v>
+      </c>
+      <c r="F66">
+        <v>236.64400000000001</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B67">
+        <v>830</v>
+      </c>
+      <c r="C67">
+        <v>24658</v>
+      </c>
+      <c r="D67">
+        <v>222.06700000000001</v>
+      </c>
+      <c r="E67">
+        <v>25537</v>
+      </c>
+      <c r="F67">
+        <v>237.05500000000001</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B68">
+        <v>840</v>
+      </c>
+      <c r="C68">
+        <v>24974</v>
+      </c>
+      <c r="D68">
+        <v>222.447</v>
+      </c>
+      <c r="E68">
+        <v>25877</v>
+      </c>
+      <c r="F68">
+        <v>237.46199999999999</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B69">
+        <v>850</v>
+      </c>
+      <c r="C69">
+        <v>25292</v>
+      </c>
+      <c r="D69">
+        <v>222.822</v>
+      </c>
+      <c r="E69">
+        <v>26218</v>
+      </c>
+      <c r="F69">
+        <v>237.864</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B70">
+        <v>860</v>
+      </c>
+      <c r="C70">
+        <v>25610</v>
+      </c>
+      <c r="D70">
+        <v>223.19399999999999</v>
+      </c>
+      <c r="E70">
+        <v>26559</v>
+      </c>
+      <c r="F70">
+        <v>238.26400000000001</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B71">
+        <v>870</v>
+      </c>
+      <c r="C71">
+        <v>25928</v>
+      </c>
+      <c r="D71">
+        <v>223.56200000000001</v>
+      </c>
+      <c r="E71">
+        <v>26899</v>
+      </c>
+      <c r="F71">
+        <v>238.66</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B72">
+        <v>880</v>
+      </c>
+      <c r="C72">
+        <v>26248</v>
+      </c>
+      <c r="D72">
+        <v>223.92699999999999</v>
+      </c>
+      <c r="E72">
+        <v>27242</v>
+      </c>
+      <c r="F72">
+        <v>239.05099999999999</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B73">
+        <v>890</v>
+      </c>
+      <c r="C73">
+        <v>26568</v>
+      </c>
+      <c r="D73">
+        <v>224.28800000000001</v>
+      </c>
+      <c r="E73">
+        <v>27584</v>
+      </c>
+      <c r="F73">
+        <v>239.43899999999999</v>
+      </c>
+    </row>
+    <row r="74" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B74">
+        <v>900</v>
+      </c>
+      <c r="C74">
+        <v>26890</v>
+      </c>
+      <c r="D74">
+        <v>224.64699999999999</v>
+      </c>
+      <c r="E74">
+        <v>27928</v>
+      </c>
+      <c r="F74">
+        <v>239.82300000000001</v>
+      </c>
+    </row>
+    <row r="75" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B75">
+        <v>910</v>
+      </c>
+      <c r="C75">
+        <v>27210</v>
+      </c>
+      <c r="D75">
+        <v>225.00200000000001</v>
+      </c>
+      <c r="E75">
+        <v>28272</v>
+      </c>
+      <c r="F75">
+        <v>240.203</v>
+      </c>
+    </row>
+    <row r="76" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B76">
+        <v>920</v>
+      </c>
+      <c r="C76">
+        <v>27532</v>
+      </c>
+      <c r="D76">
+        <v>225.35300000000001</v>
+      </c>
+      <c r="E76">
+        <v>28616</v>
+      </c>
+      <c r="F76">
+        <v>240.58</v>
+      </c>
+    </row>
+    <row r="77" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B77">
+        <v>930</v>
+      </c>
+      <c r="C77">
+        <v>27854</v>
+      </c>
+      <c r="D77">
+        <v>225.70099999999999</v>
+      </c>
+      <c r="E77">
+        <v>28960</v>
+      </c>
+      <c r="F77">
+        <v>240.953</v>
+      </c>
+    </row>
+    <row r="78" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B78">
+        <v>940</v>
+      </c>
+      <c r="C78">
+        <v>28178</v>
+      </c>
+      <c r="D78">
+        <v>226.047</v>
+      </c>
+      <c r="E78">
+        <v>29306</v>
+      </c>
+      <c r="F78">
+        <v>241.32300000000001</v>
+      </c>
+    </row>
+    <row r="79" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B79">
+        <v>950</v>
+      </c>
+      <c r="C79">
+        <v>28501</v>
+      </c>
+      <c r="D79">
+        <v>226.38900000000001</v>
+      </c>
+      <c r="E79">
+        <v>29652</v>
+      </c>
+      <c r="F79">
+        <v>241.68899999999999</v>
+      </c>
+    </row>
+    <row r="80" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B80">
+        <v>960</v>
+      </c>
+      <c r="C80">
+        <v>28826</v>
+      </c>
+      <c r="D80">
+        <v>226.72800000000001</v>
+      </c>
+      <c r="E80">
+        <v>29999</v>
+      </c>
+      <c r="F80">
+        <v>242.05199999999999</v>
+      </c>
+    </row>
+    <row r="81" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B81">
+        <v>970</v>
+      </c>
+      <c r="C81">
+        <v>29151</v>
+      </c>
+      <c r="D81">
+        <v>227.06399999999999</v>
+      </c>
+      <c r="E81">
+        <v>30345</v>
+      </c>
+      <c r="F81">
+        <v>242.411</v>
+      </c>
+    </row>
+    <row r="82" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B82">
+        <v>980</v>
+      </c>
+      <c r="C82">
+        <v>29476</v>
+      </c>
+      <c r="D82">
+        <v>227.398</v>
+      </c>
+      <c r="E82">
+        <v>30692</v>
+      </c>
+      <c r="F82">
+        <v>242.768</v>
+      </c>
+    </row>
+    <row r="83" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B83">
+        <v>990</v>
+      </c>
+      <c r="C83">
+        <v>29803</v>
+      </c>
+      <c r="D83">
+        <v>227.72800000000001</v>
+      </c>
+      <c r="E83">
+        <v>31041</v>
+      </c>
+      <c r="F83">
+        <v>243.12</v>
+      </c>
+    </row>
+    <row r="84" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B84">
+        <v>1000</v>
+      </c>
+      <c r="C84">
+        <v>30129</v>
+      </c>
+      <c r="D84">
+        <v>228.05699999999999</v>
+      </c>
+      <c r="E84">
+        <v>31389</v>
+      </c>
+      <c r="F84">
+        <v>243.471</v>
+      </c>
+    </row>
+    <row r="85" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B85">
+        <v>1020</v>
+      </c>
+      <c r="C85">
+        <v>30784</v>
+      </c>
+      <c r="D85">
+        <v>228.70599999999999</v>
+      </c>
+      <c r="E85">
+        <v>32088</v>
+      </c>
+      <c r="F85">
+        <v>244.16399999999999</v>
+      </c>
+    </row>
+    <row r="86" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B86">
+        <v>1040</v>
+      </c>
+      <c r="C86">
+        <v>31442</v>
+      </c>
+      <c r="D86">
+        <v>229.34399999999999</v>
+      </c>
+      <c r="E86">
+        <v>32789</v>
+      </c>
+      <c r="F86">
+        <v>244.84399999999999</v>
+      </c>
+    </row>
+    <row r="87" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B87">
+        <v>1060</v>
+      </c>
+      <c r="C87">
+        <v>32101</v>
+      </c>
+      <c r="D87">
+        <v>229.97300000000001</v>
+      </c>
+      <c r="E87">
+        <v>33490</v>
+      </c>
+      <c r="F87">
+        <v>245.51300000000001</v>
+      </c>
+    </row>
+    <row r="88" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B88">
+        <v>1080</v>
+      </c>
+      <c r="C88">
+        <v>32762</v>
+      </c>
+      <c r="D88">
+        <v>230.59100000000001</v>
+      </c>
+      <c r="E88">
+        <v>34194</v>
+      </c>
+      <c r="F88">
+        <v>246.17099999999999</v>
+      </c>
+    </row>
+    <row r="89" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B89">
+        <v>1100</v>
+      </c>
+      <c r="C89">
+        <v>33426</v>
+      </c>
+      <c r="D89">
+        <v>231.19900000000001</v>
+      </c>
+      <c r="E89">
+        <v>34899</v>
+      </c>
+      <c r="F89">
+        <v>246.81800000000001</v>
+      </c>
+    </row>
+    <row r="90" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B90">
+        <v>1120</v>
+      </c>
+      <c r="C90">
+        <v>34092</v>
+      </c>
+      <c r="D90">
+        <v>231.79900000000001</v>
+      </c>
+      <c r="E90">
+        <v>35606</v>
+      </c>
+      <c r="F90">
+        <v>247.45400000000001</v>
+      </c>
+    </row>
+    <row r="91" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B91">
+        <v>1140</v>
+      </c>
+      <c r="C91">
+        <v>34760</v>
+      </c>
+      <c r="D91">
+        <v>232.39099999999999</v>
+      </c>
+      <c r="E91">
+        <v>36314</v>
+      </c>
+      <c r="F91">
+        <v>248.08099999999999</v>
+      </c>
+    </row>
+    <row r="92" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B92">
+        <v>1160</v>
+      </c>
+      <c r="C92">
+        <v>35430</v>
+      </c>
+      <c r="D92">
+        <v>232.97300000000001</v>
+      </c>
+      <c r="E92">
+        <v>37023</v>
+      </c>
+      <c r="F92">
+        <v>248.69800000000001</v>
+      </c>
+    </row>
+    <row r="93" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B93">
+        <v>1180</v>
+      </c>
+      <c r="C93">
+        <v>36104</v>
+      </c>
+      <c r="D93">
+        <v>233.54900000000001</v>
+      </c>
+      <c r="E93">
+        <v>37734</v>
+      </c>
+      <c r="F93">
+        <v>249.30699999999999</v>
+      </c>
+    </row>
+    <row r="94" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B94">
+        <v>1200</v>
+      </c>
+      <c r="C94">
+        <v>36777</v>
+      </c>
+      <c r="D94">
+        <v>234.11500000000001</v>
+      </c>
+      <c r="E94">
+        <v>38447</v>
+      </c>
+      <c r="F94">
+        <v>249.90600000000001</v>
+      </c>
+    </row>
+    <row r="95" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B95">
+        <v>1220</v>
+      </c>
+      <c r="C95">
+        <v>37452</v>
+      </c>
+      <c r="D95">
+        <v>234.673</v>
+      </c>
+      <c r="E95">
+        <v>39162</v>
+      </c>
+      <c r="F95">
+        <v>250.49700000000001</v>
+      </c>
+    </row>
+    <row r="96" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B96">
+        <v>1240</v>
+      </c>
+      <c r="C96">
+        <v>38129</v>
+      </c>
+      <c r="D96">
+        <v>235.22300000000001</v>
+      </c>
+      <c r="E96">
+        <v>39877</v>
+      </c>
+      <c r="F96">
+        <v>251.07900000000001</v>
+      </c>
+    </row>
+    <row r="97" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B97">
+        <v>1260</v>
+      </c>
+      <c r="C97">
+        <v>38807</v>
+      </c>
+      <c r="D97">
+        <v>235.76599999999999</v>
+      </c>
+      <c r="E97">
+        <v>40594</v>
+      </c>
+      <c r="F97">
+        <v>251.65299999999999</v>
+      </c>
+    </row>
+    <row r="98" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B98">
+        <v>1280</v>
+      </c>
+      <c r="C98">
+        <v>39488</v>
+      </c>
+      <c r="D98">
+        <v>236.30199999999999</v>
+      </c>
+      <c r="E98">
+        <v>41312</v>
+      </c>
+      <c r="F98">
+        <v>252.21899999999999</v>
+      </c>
+    </row>
+    <row r="99" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B99">
+        <v>1300</v>
+      </c>
+      <c r="C99">
+        <v>40170</v>
+      </c>
+      <c r="D99">
+        <v>236.83099999999999</v>
+      </c>
+      <c r="E99">
+        <v>42033</v>
+      </c>
+      <c r="F99">
+        <v>252.77600000000001</v>
+      </c>
+    </row>
+    <row r="100" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B100">
+        <v>1320</v>
+      </c>
+      <c r="C100">
+        <v>40853</v>
+      </c>
+      <c r="D100">
+        <v>237.35300000000001</v>
+      </c>
+      <c r="E100">
+        <v>42753</v>
+      </c>
+      <c r="F100">
+        <v>253.32499999999999</v>
+      </c>
+    </row>
+    <row r="101" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B101">
+        <v>1340</v>
+      </c>
+      <c r="C101">
+        <v>41539</v>
+      </c>
+      <c r="D101">
+        <v>237.86699999999999</v>
+      </c>
+      <c r="E101">
+        <v>43475</v>
+      </c>
+      <c r="F101">
+        <v>253.86799999999999</v>
+      </c>
+    </row>
+    <row r="102" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B102">
+        <v>1360</v>
+      </c>
+      <c r="C102">
+        <v>42227</v>
+      </c>
+      <c r="D102">
+        <v>238.376</v>
+      </c>
+      <c r="E102">
+        <v>44198</v>
+      </c>
+      <c r="F102">
+        <v>254.404</v>
+      </c>
+    </row>
+    <row r="103" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B103">
+        <v>1380</v>
+      </c>
+      <c r="C103">
+        <v>42915</v>
+      </c>
+      <c r="D103">
+        <v>238.87799999999999</v>
+      </c>
+      <c r="E103">
+        <v>44923</v>
+      </c>
+      <c r="F103">
+        <v>254.93199999999999</v>
+      </c>
+    </row>
+    <row r="104" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B104">
+        <v>1400</v>
+      </c>
+      <c r="C104">
+        <v>43605</v>
+      </c>
+      <c r="D104">
+        <v>239.375</v>
+      </c>
+      <c r="E104">
+        <v>45648</v>
+      </c>
+      <c r="F104">
+        <v>255.45400000000001</v>
+      </c>
+    </row>
+    <row r="105" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B105">
+        <v>1420</v>
+      </c>
+      <c r="C105">
+        <v>44295</v>
+      </c>
+      <c r="D105">
+        <v>239.86500000000001</v>
+      </c>
+      <c r="E105">
+        <v>46374</v>
+      </c>
+      <c r="F105">
+        <v>255.96799999999999</v>
+      </c>
+    </row>
+    <row r="106" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B106">
+        <v>1440</v>
+      </c>
+      <c r="C106">
+        <v>44988</v>
+      </c>
+      <c r="D106">
+        <v>240.35</v>
+      </c>
+      <c r="E106">
+        <v>47102</v>
+      </c>
+      <c r="F106">
+        <v>256.47500000000002</v>
+      </c>
+    </row>
+    <row r="107" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B107">
+        <v>1460</v>
+      </c>
+      <c r="C107">
+        <v>45682</v>
+      </c>
+      <c r="D107">
+        <v>240.827</v>
+      </c>
+      <c r="E107">
+        <v>47831</v>
+      </c>
+      <c r="F107">
+        <v>256.97800000000001</v>
+      </c>
+    </row>
+    <row r="108" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B108">
+        <v>1480</v>
+      </c>
+      <c r="C108">
+        <v>46377</v>
+      </c>
+      <c r="D108">
+        <v>241.30099999999999</v>
+      </c>
+      <c r="E108">
+        <v>48561</v>
+      </c>
+      <c r="F108">
+        <v>257.47399999999999</v>
+      </c>
+    </row>
+    <row r="109" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B109">
+        <v>1500</v>
+      </c>
+      <c r="C109">
+        <v>47073</v>
+      </c>
+      <c r="D109">
+        <v>241.768</v>
+      </c>
+      <c r="E109">
+        <v>49292</v>
+      </c>
+      <c r="F109">
+        <v>257.96499999999997</v>
+      </c>
+    </row>
+    <row r="110" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B110">
+        <v>1520</v>
+      </c>
+      <c r="C110">
+        <v>47771</v>
+      </c>
+      <c r="D110">
+        <v>242.22800000000001</v>
+      </c>
+      <c r="E110">
+        <v>50024</v>
+      </c>
+      <c r="F110">
+        <v>258.45</v>
+      </c>
+    </row>
+    <row r="111" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B111">
+        <v>1540</v>
+      </c>
+      <c r="C111">
+        <v>48470</v>
+      </c>
+      <c r="D111">
+        <v>242.685</v>
+      </c>
+      <c r="E111">
+        <v>50756</v>
+      </c>
+      <c r="F111">
+        <v>258.928</v>
+      </c>
+    </row>
+    <row r="112" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B112">
+        <v>1560</v>
+      </c>
+      <c r="C112">
+        <v>49168</v>
+      </c>
+      <c r="D112">
+        <v>243.137</v>
+      </c>
+      <c r="E112">
+        <v>51490</v>
+      </c>
+      <c r="F112">
+        <v>259.40199999999999</v>
+      </c>
+    </row>
+    <row r="113" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B113">
+        <v>1580</v>
+      </c>
+      <c r="C113">
+        <v>49869</v>
+      </c>
+      <c r="D113">
+        <v>243.58500000000001</v>
+      </c>
+      <c r="E113">
+        <v>52224</v>
+      </c>
+      <c r="F113">
+        <v>259.87</v>
+      </c>
+    </row>
+    <row r="114" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B114">
+        <v>1600</v>
+      </c>
+      <c r="C114">
+        <v>50571</v>
+      </c>
+      <c r="D114">
+        <v>244.02799999999999</v>
+      </c>
+      <c r="E114">
+        <v>52961</v>
+      </c>
+      <c r="F114">
+        <v>260.33300000000003</v>
+      </c>
+    </row>
+    <row r="115" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B115">
+        <v>1620</v>
+      </c>
+      <c r="C115">
+        <v>51275</v>
+      </c>
+      <c r="D115">
+        <v>244.464</v>
+      </c>
+      <c r="E115">
+        <v>53696</v>
+      </c>
+      <c r="F115">
+        <v>260.791</v>
+      </c>
+    </row>
+    <row r="116" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B116">
+        <v>1640</v>
+      </c>
+      <c r="C116">
+        <v>51980</v>
+      </c>
+      <c r="D116">
+        <v>244.89599999999999</v>
+      </c>
+      <c r="E116">
+        <v>54434</v>
+      </c>
+      <c r="F116">
+        <v>261.24200000000002</v>
+      </c>
+    </row>
+    <row r="117" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B117">
+        <v>1660</v>
+      </c>
+      <c r="C117">
+        <v>52686</v>
+      </c>
+      <c r="D117">
+        <v>245.32400000000001</v>
+      </c>
+      <c r="E117">
+        <v>55172</v>
+      </c>
+      <c r="F117">
+        <v>261.69</v>
+      </c>
+    </row>
+    <row r="118" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B118">
+        <v>1680</v>
+      </c>
+      <c r="C118">
+        <v>53393</v>
+      </c>
+      <c r="D118">
+        <v>245.74700000000001</v>
+      </c>
+      <c r="E118">
+        <v>55912</v>
+      </c>
+      <c r="F118">
+        <v>262.13200000000001</v>
+      </c>
+    </row>
+    <row r="119" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B119">
+        <v>1700</v>
+      </c>
+      <c r="C119">
+        <v>54099</v>
+      </c>
+      <c r="D119">
+        <v>246.166</v>
+      </c>
+      <c r="E119">
+        <v>56652</v>
+      </c>
+      <c r="F119">
+        <v>262.57100000000003</v>
+      </c>
+    </row>
+    <row r="120" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B120">
+        <v>1720</v>
+      </c>
+      <c r="C120">
+        <v>54807</v>
+      </c>
+      <c r="D120">
+        <v>246.58</v>
+      </c>
+      <c r="E120">
+        <v>57394</v>
+      </c>
+      <c r="F120">
+        <v>263.005</v>
+      </c>
+    </row>
+    <row r="121" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B121">
+        <v>1740</v>
+      </c>
+      <c r="C121">
+        <v>55516</v>
+      </c>
+      <c r="D121">
+        <v>246.99</v>
+      </c>
+      <c r="E121">
+        <v>58136</v>
+      </c>
+      <c r="F121">
+        <v>263.435</v>
+      </c>
+    </row>
+    <row r="122" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B122">
+        <v>1760</v>
+      </c>
+      <c r="C122">
+        <v>56227</v>
+      </c>
+      <c r="D122">
+        <v>247.39599999999999</v>
+      </c>
+      <c r="E122">
+        <v>58800</v>
+      </c>
+      <c r="F122">
+        <v>263.86099999999999</v>
+      </c>
+    </row>
+    <row r="123" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B123">
+        <v>1780</v>
+      </c>
+      <c r="C123">
+        <v>56938</v>
+      </c>
+      <c r="D123">
+        <v>247.798</v>
+      </c>
+      <c r="E123">
+        <v>59624</v>
+      </c>
+      <c r="F123">
+        <v>264.28300000000002</v>
+      </c>
+    </row>
+    <row r="124" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B124">
+        <v>1800</v>
+      </c>
+      <c r="C124">
+        <v>57651</v>
+      </c>
+      <c r="D124">
+        <v>248.19499999999999</v>
+      </c>
+      <c r="E124">
+        <v>60371</v>
+      </c>
+      <c r="F124">
+        <v>264.70100000000002</v>
+      </c>
+    </row>
+    <row r="125" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B125">
+        <v>1820</v>
+      </c>
+      <c r="C125">
+        <v>58363</v>
+      </c>
+      <c r="D125">
+        <v>248.589</v>
+      </c>
+      <c r="E125">
+        <v>61118</v>
+      </c>
+      <c r="F125">
+        <v>265.113</v>
+      </c>
+    </row>
+    <row r="126" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B126">
+        <v>1840</v>
+      </c>
+      <c r="C126">
+        <v>59075</v>
+      </c>
+      <c r="D126">
+        <v>248.97900000000001</v>
+      </c>
+      <c r="E126">
+        <v>61866</v>
+      </c>
+      <c r="F126">
+        <v>265.52100000000002</v>
+      </c>
+    </row>
+    <row r="127" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B127">
+        <v>1860</v>
+      </c>
+      <c r="C127">
+        <v>59790</v>
+      </c>
+      <c r="D127">
+        <v>249.36500000000001</v>
+      </c>
+      <c r="E127">
+        <v>62616</v>
+      </c>
+      <c r="F127">
+        <v>265.92500000000001</v>
+      </c>
+    </row>
+    <row r="128" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B128">
+        <v>1880</v>
+      </c>
+      <c r="C128">
+        <v>60504</v>
+      </c>
+      <c r="D128">
+        <v>249.74799999999999</v>
+      </c>
+      <c r="E128">
+        <v>63365</v>
+      </c>
+      <c r="F128">
+        <v>266.32600000000002</v>
+      </c>
+    </row>
+    <row r="129" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B129">
+        <v>1900</v>
+      </c>
+      <c r="C129">
+        <v>61220</v>
+      </c>
+      <c r="D129">
+        <v>250.12799999999999</v>
+      </c>
+      <c r="E129">
+        <v>64116</v>
+      </c>
+      <c r="F129">
+        <v>266.72199999999998</v>
+      </c>
+    </row>
+    <row r="130" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B130">
+        <v>1920</v>
+      </c>
+      <c r="C130">
+        <v>61936</v>
+      </c>
+      <c r="D130">
+        <v>250.50200000000001</v>
+      </c>
+      <c r="E130">
+        <v>64868</v>
+      </c>
+      <c r="F130">
+        <v>267.11500000000001</v>
+      </c>
+    </row>
+    <row r="131" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B131">
+        <v>1940</v>
+      </c>
+      <c r="C131">
+        <v>62654</v>
+      </c>
+      <c r="D131">
+        <v>250.874</v>
+      </c>
+      <c r="E131">
+        <v>65620</v>
+      </c>
+      <c r="F131">
+        <v>267.505</v>
+      </c>
+    </row>
+    <row r="132" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B132">
+        <v>1960</v>
+      </c>
+      <c r="C132">
+        <v>63381</v>
+      </c>
+      <c r="D132">
+        <v>251.24199999999999</v>
+      </c>
+      <c r="E132">
+        <v>66374</v>
+      </c>
+      <c r="F132">
+        <v>267.89100000000002</v>
+      </c>
+    </row>
+    <row r="133" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B133">
+        <v>1980</v>
+      </c>
+      <c r="C133">
+        <v>64090</v>
+      </c>
+      <c r="D133">
+        <v>251.607</v>
+      </c>
+      <c r="E133">
+        <v>67127</v>
+      </c>
+      <c r="F133">
+        <v>268.27499999999998</v>
+      </c>
+    </row>
+    <row r="134" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B134">
+        <v>2000</v>
+      </c>
+      <c r="C134">
+        <v>64810</v>
+      </c>
+      <c r="D134">
+        <v>251.96899999999999</v>
+      </c>
+      <c r="E134">
+        <v>67881</v>
+      </c>
+      <c r="F134">
+        <v>268.65499999999997</v>
+      </c>
+    </row>
+    <row r="135" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B135">
+        <v>2050</v>
+      </c>
+      <c r="C135">
+        <v>66612</v>
+      </c>
+      <c r="D135">
+        <v>252.858</v>
+      </c>
+      <c r="E135">
+        <v>69772</v>
+      </c>
+      <c r="F135">
+        <v>269.58800000000002</v>
+      </c>
+    </row>
+    <row r="136" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B136">
+        <v>2100</v>
+      </c>
+      <c r="C136">
+        <v>68417</v>
+      </c>
+      <c r="D136">
+        <v>253.726</v>
+      </c>
+      <c r="E136">
+        <v>71668</v>
+      </c>
+      <c r="F136">
+        <v>270.50400000000002</v>
+      </c>
+    </row>
+    <row r="137" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B137">
+        <v>2150</v>
+      </c>
+      <c r="C137">
+        <v>70226</v>
+      </c>
+      <c r="D137">
+        <v>254.578</v>
+      </c>
+      <c r="E137">
+        <v>73573</v>
+      </c>
+      <c r="F137">
+        <v>271.399</v>
+      </c>
+    </row>
+    <row r="138" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B138">
+        <v>2200</v>
+      </c>
+      <c r="C138">
+        <v>72040</v>
+      </c>
+      <c r="D138">
+        <v>255.41200000000001</v>
+      </c>
+      <c r="E138">
+        <v>75484</v>
+      </c>
+      <c r="F138">
+        <v>272.27800000000002</v>
+      </c>
+    </row>
+    <row r="139" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B139">
+        <v>2250</v>
+      </c>
+      <c r="C139">
+        <v>73856</v>
+      </c>
+      <c r="D139">
+        <v>256.22699999999998</v>
+      </c>
+      <c r="E139">
+        <v>77397</v>
+      </c>
+      <c r="F139">
+        <v>273.13600000000002</v>
+      </c>
+    </row>
+    <row r="140" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B140">
+        <v>2300</v>
+      </c>
+      <c r="C140">
+        <v>75676</v>
+      </c>
+      <c r="D140">
+        <v>257.02699999999999</v>
+      </c>
+      <c r="E140">
+        <v>79316</v>
+      </c>
+      <c r="F140">
+        <v>273.98099999999999</v>
+      </c>
+    </row>
+    <row r="141" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B141">
+        <v>2350</v>
+      </c>
+      <c r="C141">
+        <v>77496</v>
+      </c>
+      <c r="D141">
+        <v>257.81</v>
+      </c>
+      <c r="E141">
+        <v>81243</v>
+      </c>
+      <c r="F141">
+        <v>274.80900000000003</v>
+      </c>
+    </row>
+    <row r="142" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B142">
+        <v>2400</v>
+      </c>
+      <c r="C142">
+        <v>79320</v>
+      </c>
+      <c r="D142">
+        <v>258.58</v>
+      </c>
+      <c r="E142">
+        <v>83474</v>
+      </c>
+      <c r="F142">
+        <v>275.625</v>
+      </c>
+    </row>
+    <row r="143" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B143">
+        <v>2450</v>
+      </c>
+      <c r="C143">
+        <v>81149</v>
+      </c>
+      <c r="D143">
+        <v>259.33199999999999</v>
+      </c>
+      <c r="E143">
+        <v>85112</v>
+      </c>
+      <c r="F143">
+        <v>276.42399999999998</v>
+      </c>
+    </row>
+    <row r="144" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B144">
+        <v>2500</v>
+      </c>
+      <c r="C144">
+        <v>82981</v>
+      </c>
+      <c r="D144">
+        <v>260.07299999999998</v>
+      </c>
+      <c r="E144">
+        <v>87057</v>
+      </c>
+      <c r="F144">
+        <v>277.20699999999999</v>
+      </c>
+    </row>
+    <row r="145" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B145">
+        <v>2550</v>
+      </c>
+      <c r="C145">
+        <v>84814</v>
+      </c>
+      <c r="D145">
+        <v>260.79899999999998</v>
+      </c>
+      <c r="E145">
+        <v>89004</v>
+      </c>
+      <c r="F145">
+        <v>277.97899999999998</v>
+      </c>
+    </row>
+    <row r="146" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B146">
+        <v>2600</v>
+      </c>
+      <c r="C146">
+        <v>86650</v>
+      </c>
+      <c r="D146">
+        <v>261.512</v>
+      </c>
+      <c r="E146">
+        <v>90956</v>
+      </c>
+      <c r="F146">
+        <v>278.738</v>
+      </c>
+    </row>
+    <row r="147" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B147">
+        <v>2650</v>
+      </c>
+      <c r="C147">
+        <v>88488</v>
+      </c>
+      <c r="D147">
+        <v>262.21300000000002</v>
+      </c>
+      <c r="E147">
+        <v>92916</v>
+      </c>
+      <c r="F147">
+        <v>279.48500000000001</v>
+      </c>
+    </row>
+    <row r="148" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B148">
+        <v>2700</v>
+      </c>
+      <c r="C148">
+        <v>90328</v>
+      </c>
+      <c r="D148">
+        <v>262.90199999999999</v>
+      </c>
+      <c r="E148">
+        <v>94881</v>
+      </c>
+      <c r="F148">
+        <v>280.21899999999999</v>
+      </c>
+    </row>
+    <row r="149" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B149">
+        <v>2750</v>
+      </c>
+      <c r="C149">
+        <v>92171</v>
+      </c>
+      <c r="D149">
+        <v>263.577</v>
+      </c>
+      <c r="E149">
+        <v>96852</v>
+      </c>
+      <c r="F149">
+        <v>280.94200000000001</v>
+      </c>
+    </row>
+    <row r="150" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B150">
+        <v>2800</v>
+      </c>
+      <c r="C150">
+        <v>94014</v>
+      </c>
+      <c r="D150">
+        <v>264.24099999999999</v>
+      </c>
+      <c r="E150">
+        <v>98826</v>
+      </c>
+      <c r="F150">
+        <v>281.654</v>
+      </c>
+    </row>
+    <row r="151" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B151">
+        <v>2850</v>
+      </c>
+      <c r="C151">
+        <v>95859</v>
+      </c>
+      <c r="D151">
+        <v>264.89499999999998</v>
+      </c>
+      <c r="E151">
+        <v>100808</v>
+      </c>
+      <c r="F151">
+        <v>282.35700000000003</v>
+      </c>
+    </row>
+    <row r="152" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B152">
+        <v>2900</v>
+      </c>
+      <c r="C152">
+        <v>97705</v>
+      </c>
+      <c r="D152">
+        <v>265.53800000000001</v>
+      </c>
+      <c r="E152">
+        <v>102793</v>
+      </c>
+      <c r="F152">
+        <v>283.048</v>
+      </c>
+    </row>
+    <row r="153" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B153">
+        <v>2950</v>
+      </c>
+      <c r="C153">
+        <v>99556</v>
+      </c>
+      <c r="D153">
+        <v>266.17</v>
+      </c>
+      <c r="E153">
+        <v>104785</v>
+      </c>
+      <c r="F153">
+        <v>283.72800000000001</v>
+      </c>
+    </row>
+    <row r="154" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B154">
+        <v>3000</v>
+      </c>
+      <c r="C154">
+        <v>101407</v>
+      </c>
+      <c r="D154">
+        <v>266.79300000000001</v>
+      </c>
+      <c r="E154">
+        <v>106780</v>
+      </c>
+      <c r="F154">
+        <v>284.399</v>
+      </c>
+    </row>
+    <row r="155" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B155">
+        <v>3050</v>
+      </c>
+      <c r="C155">
+        <v>103260</v>
+      </c>
+      <c r="D155">
+        <v>267.404</v>
+      </c>
+      <c r="E155">
+        <v>108778</v>
+      </c>
+      <c r="F155">
+        <v>285.06</v>
+      </c>
+    </row>
+    <row r="156" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B156">
+        <v>3100</v>
+      </c>
+      <c r="C156">
+        <v>105115</v>
+      </c>
+      <c r="D156">
+        <v>268.00700000000001</v>
+      </c>
+      <c r="E156">
+        <v>110784</v>
+      </c>
+      <c r="F156">
+        <v>285.71300000000002</v>
+      </c>
+    </row>
+    <row r="157" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B157">
+        <v>3150</v>
+      </c>
+      <c r="C157">
+        <v>106972</v>
+      </c>
+      <c r="D157">
+        <v>268.601</v>
+      </c>
+      <c r="E157">
+        <v>112795</v>
+      </c>
+      <c r="F157">
+        <v>286.35500000000002</v>
+      </c>
+    </row>
+    <row r="158" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B158">
         <v>3200</v>
       </c>
-      <c r="C41">
+      <c r="C158">
         <v>108830</v>
       </c>
-      <c r="D41">
+      <c r="D158">
         <v>269.18599999999998</v>
       </c>
-      <c r="E41">
+      <c r="E158">
         <v>114809</v>
       </c>
-      <c r="F41">
+      <c r="F158">
         <v>286.98899999999998</v>
+      </c>
+    </row>
+    <row r="159" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B159">
+        <v>3250</v>
+      </c>
+      <c r="C159">
+        <v>110690</v>
+      </c>
+      <c r="D159">
+        <v>269.76299999999998</v>
+      </c>
+      <c r="E159">
+        <v>116827</v>
+      </c>
+      <c r="F159">
+        <v>287.61399999999998</v>
       </c>
     </row>
   </sheetData>
@@ -4107,6 +6109,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000E094FB6986D7A449CDA976CB7BB2E51" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8f658ff9f332929447915d87901a0080">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="7f3ca868-b031-4e60-87f4-a1bfe4f2ec3c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b16dcfd7401e56f85c56a035f11e472a" ns3:_="">
     <xsd:import namespace="7f3ca868-b031-4e60-87f4-a1bfe4f2ec3c"/>
@@ -4302,15 +6313,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{796A5BBF-1CA1-4B58-BB05-F028BCC8BF96}">
   <ds:schemaRefs>
@@ -4328,6 +6330,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E00589F-6A95-404C-9940-B281A1AB26E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0D1E3DD-BA62-4675-8C41-74D388E9AC87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4343,12 +6353,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E00589F-6A95-404C-9940-B281A1AB26E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>